<commit_message>
Update Third Normal Form Worksheet_Automobile_Club_Completed.xlsx
</commit_message>
<xml_diff>
--- a/Chapter02/Activity 2/Third Normal Form Worksheet_Automobile_Club_Completed.xlsx
+++ b/Chapter02/Activity 2/Third Normal Form Worksheet_Automobile_Club_Completed.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B9BA08-83FC-489A-8239-04A5A721BCAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Drivers License" sheetId="1" r:id="rId1"/>
@@ -425,7 +426,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -557,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -580,9 +581,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -689,6 +687,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -724,6 +739,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -899,11 +931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,203 +991,203 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>37</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>15</v>
@@ -1164,48 +1196,48 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="B19" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>48</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
@@ -1213,13 +1245,13 @@
         <v>14</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1228,98 +1260,101 @@
         <v>14</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>33</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="7" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="7" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="7" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E26">
+    <sortCondition ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1787,17 +1822,17 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="57" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13" t="s">
+      <c r="A30" s="11"/>
+      <c r="B30" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="12" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>